<commit_message>
both: login and register
</commit_message>
<xml_diff>
--- a/doc/backend api.xlsx
+++ b/doc/backend api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KUJO JOTARO\Desktop\github\nest-bs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4415BD0B-3309-465B-B651-0B94294E79D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A577E8F8-FB10-42AE-A6E1-3885294F27D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E1DD6AB-21D5-4F64-B824-AD98C978794E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>user.controller.ts</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,10 +136,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>200，user对象, register_success,register_failed,wrong_mail_code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/changepwd/:mail/:code/:pwd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -149,6 +145,18 @@
   </si>
   <si>
     <t>200,change_pwd_susscess,change_pwd_failed,wrong_mail_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200，user对象, register_success,register_failed,wrong_mail_code,user_exists</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询用户是否存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改密码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -519,7 +527,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -596,7 +604,7 @@
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
@@ -632,19 +640,25 @@
       <c r="E6" t="s">
         <v>24</v>
       </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
+      <c r="F7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>